<commit_message>
Multiple updates based on Dr. K comments.
Updated models, updated writeup, updated method of param serches.
Please look at Exercise4_RFCMLP.ipynb for Code, and ExerciseR.pdf for writeup.
</commit_message>
<xml_diff>
--- a/performance_scores.xlsx
+++ b/performance_scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,116 +473,116 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BayesSearchCV</t>
+          <t>GridSearchCV</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.987489574645538</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6522448979591837</v>
+        <v>0.63</v>
       </c>
       <c r="D2" t="n">
-        <v>76.11753582954407</v>
+        <v>6.917701244354248</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6743861795399358</v>
+        <v>0.6522280334728033</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Full Train Set</t>
+          <t>Full Dataset</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>OrderedDict([('bootstrap', True), ('criterion', 'entropy'), ('max_depth', None), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', False)])</t>
+          <t>{'bootstrap': True, 'bootstrap_features': False, 'n_estimators': 10, 'n_jobs': -1, 'random_state': 1, 'verbose': True}</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BayesSearchCV</t>
+          <t>GridSearchCV</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.987489574645538</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6848979591836735</v>
+        <v>0.63</v>
       </c>
       <c r="D3" t="n">
-        <v>66.77413725852965</v>
+        <v>17.54486274719238</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6602124228437969</v>
+        <v>0.6555509065550906</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Full Train Set</t>
+          <t>Full Dataset</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>OrderedDict([('bootstrap', True), ('criterion', 'log_loss'), ('max_depth', 25), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', False)])</t>
+          <t>{'bootstrap': True, 'bootstrap_features': False, 'estimator': DecisionTreeClassifier(), 'n_estimators': 10, 'n_jobs': -1, 'random_state': None, 'verbose': True}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RandomizedSearchCV</t>
+          <t>GridSearchCV</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0.6021684737281068</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6636734693877551</v>
+        <v>0.555</v>
       </c>
       <c r="D4" t="n">
-        <v>11.91021585464478</v>
+        <v>225.9832837581635</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6648568092086972</v>
+        <v>0.5971966527196653</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Full Train Set</t>
+          <t>Full Dataset</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>{'warm_start': False, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': 25, 'criterion': 'gini', 'bootstrap': False}</t>
+          <t>{'bootstrap': True, 'bootstrap_features': True, 'estimator': DecisionTreeClassifier(), 'max_samples': 25, 'n_estimators': 25, 'n_jobs': -1, 'random_state': 100, 'verbose': True}</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>RandomizedSearchCV</t>
+          <t>GridSearchCV</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.5239651416122004</v>
       </c>
       <c r="C5" t="n">
-        <v>0.673469387755102</v>
+        <v>0.5</v>
       </c>
       <c r="D5" t="n">
-        <v>7.67133092880249</v>
+        <v>48.73722720146178</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6583139631874548</v>
+        <v>0.5479805179377525</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Full Train Set</t>
+          <t>Full Dataset</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>{'warm_start': True, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': None, 'criterion': 'log_loss', 'bootstrap': False}</t>
+          <t>{'bootstrap': False, 'bootstrap_features': False, 'estimator': DecisionTreeClassifier(), 'max_samples': 25, 'n_estimators': 25, 'n_jobs': -1, 'random_state': 2024, 'verbose': True}</t>
         </is>
       </c>
     </row>
@@ -593,25 +593,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0.5544662309368191</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6595918367346939</v>
+        <v>0.5196078431372549</v>
       </c>
       <c r="D6" t="n">
-        <v>27.17054367065429</v>
+        <v>48.6426305770874</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6754805464420101</v>
+        <v>0.5174031836540747</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Full_Train_Set</t>
+          <t>Full Dataset</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>{'bootstrap': True, 'criterion': 'gini', 'max_depth': 25, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': False}</t>
+          <t>{'bootstrap': False, 'bootstrap_features': False, 'estimator': DecisionTreeClassifier(), 'max_samples': 25, 'n_estimators': 25, 'n_jobs': -1, 'random_state': 2024, 'verbose': True}</t>
         </is>
       </c>
     </row>
@@ -622,228 +622,228 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0.7603485838779956</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6661224489795918</v>
+        <v>0.5816993464052288</v>
       </c>
       <c r="D7" t="n">
-        <v>26.61089396476745</v>
+        <v>699.3307025432587</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6733007099297484</v>
+        <v>0.5599786172487526</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Full_Train_Set</t>
+          <t>Full Dataset</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>{'bootstrap': True, 'criterion': 'entropy', 'max_depth': 25, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': False}</t>
+          <t>{'bootstrap': True, 'bootstrap_features': False, 'estimator': DecisionTreeClassifier(), 'max_features': 11, 'max_samples': 200, 'n_estimators': 50, 'n_jobs': -1, 'random_state': 1, 'verbose': True}</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GridSearchCV</t>
+          <t>RandomizedSearchCV</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0.673202614379085</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6751020408163265</v>
+        <v>0.5326797385620915</v>
       </c>
       <c r="D8" t="n">
-        <v>28.02601218223571</v>
+        <v>39.39143705368042</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6626662218020722</v>
+        <v>0.5392254692325968</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Full_Train_Set</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>{'bootstrap': True, 'criterion': 'entropy', 'max_depth': None, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': False}</t>
+          <t>{'verbose': True, 'n_estimators': 200, 'min_weight_fraction_leaf': 0.001, 'min_samples_split': 6, 'min_samples_leaf': 1, 'max_features': 5, 'max_depth': 10, 'loss': 'log_loss', 'learning_rate': 0.1, 'init': None, 'criterion': 'squared_error'}</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BayesSearchCV</t>
+          <t>RandomizedSearchCV</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9814814814814815</v>
+        <v>0.9836601307189542</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.565359477124183</v>
       </c>
       <c r="D9" t="n">
-        <v>48.89439749717713</v>
+        <v>15.63972711563111</v>
       </c>
       <c r="E9" t="n">
-        <v>0.56535994297933</v>
+        <v>0.5511819909717273</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Meta 25%</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>OrderedDict([('bootstrap', True), ('criterion', 'entropy'), ('max_depth', 10), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', False)])</t>
+          <t>{'verbose': True, 'n_estimators': 100, 'min_weight_fraction_leaf': 0.01, 'min_samples_split': 6, 'min_samples_leaf': 1, 'max_features': 9, 'max_depth': 10, 'loss': 'log_loss', 'learning_rate': 0.1, 'init': 'zero', 'criterion': 'squared_error'}</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BayesSearchCV</t>
+          <t>RandomizedSearchCV</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9901960784313726</v>
+        <v>0.9424520433694745</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5816993464052288</v>
+        <v>0.6274999999999999</v>
       </c>
       <c r="D10" t="n">
-        <v>43.69706463813783</v>
+        <v>17.44346523284912</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5981052506533618</v>
+        <v>0.6639051603905161</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Meta 25%</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>OrderedDict([('bootstrap', True), ('criterion', 'log_loss'), ('max_depth', 10), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', False)])</t>
+          <t>{'verbose': True, 'n_estimators': 100, 'min_weight_fraction_leaf': 0.01, 'min_samples_split': 2, 'min_samples_leaf': 10, 'max_features': 5, 'max_depth': 10, 'loss': 'log_loss', 'learning_rate': 0.1, 'init': 'zero', 'criterion': 'squared_error'}</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BayesSearchCV</t>
+          <t>RandomizedSearchCV</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9673202614379085</v>
+        <v>0.7306088407005839</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5882352941176471</v>
+        <v>0.605</v>
       </c>
       <c r="D11" t="n">
-        <v>43.42147016525269</v>
+        <v>19.87313103675842</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5882988833452126</v>
+        <v>0.5888354253835425</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Meta 25%</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>OrderedDict([('bootstrap', True), ('criterion', 'gini'), ('max_depth', 10), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', False)])</t>
+          <t>{'verbose': True, 'n_estimators': 200, 'min_weight_fraction_leaf': 0.1, 'min_samples_split': 2, 'min_samples_leaf': 1, 'max_features': 5, 'max_depth': 5, 'loss': 'log_loss', 'learning_rate': 0.001, 'init': None, 'criterion': 'squared_error'}</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GridSearchCV</t>
+          <t>RandomizedSearchCV</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9814814814814815</v>
+        <v>0.6071726438698916</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.545</v>
       </c>
       <c r="D12" t="n">
-        <v>15.5570719242096</v>
+        <v>19.61344599723816</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5610180565454976</v>
+        <v>0.6647280334728034</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Meta 25%</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>{'bootstrap': True, 'criterion': 'log_loss', 'max_depth': 10, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': True}</t>
+          <t>{'verbose': True, 'n_estimators': 200, 'min_weight_fraction_leaf': 0.001, 'min_samples_split': 2, 'min_samples_leaf': 1, 'max_features': 9, 'max_depth': 3, 'loss': 'log_loss', 'learning_rate': 0.1, 'init': 'zero', 'criterion': 'squared_error'}</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GridSearchCV</t>
+          <t>RandomizedSearchCV</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9705882352941176</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5588235294117647</v>
+        <v>0.63</v>
       </c>
       <c r="D13" t="n">
-        <v>15.04339814186097</v>
+        <v>33.74400210380553</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5991803278688523</v>
+        <v>0.6563807531380753</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Meta 25%</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>{'bootstrap': True, 'criterion': 'gini', 'max_depth': 10, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': True}</t>
+          <t>{'verbose': True, 'n_estimators': 200, 'min_weight_fraction_leaf': 0.01, 'min_samples_split': 6, 'min_samples_leaf': 5, 'max_features': 11, 'max_depth': 5, 'loss': 'log_loss', 'learning_rate': 0.1, 'init': None, 'criterion': 'friedman_mse'}</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GridSearchCV</t>
+          <t>RandomizedSearchCV</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9901960784313726</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5849673202614379</v>
+        <v>0.6425</v>
       </c>
       <c r="D14" t="n">
-        <v>15.25957012176513</v>
+        <v>5.184916019439698</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5763423616060822</v>
+        <v>0.5988598326359832</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Meta 25%</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>{'bootstrap': True, 'criterion': 'entropy', 'max_depth': 10, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': False}</t>
+          <t>{'verbose': True, 'n_estimators': 100, 'min_weight_fraction_leaf': 0.1, 'min_samples_split': 2, 'min_samples_leaf': 10, 'max_features': 5, 'max_depth': 10, 'loss': 'log_loss', 'learning_rate': 0.001, 'init': 'zero', 'criterion': 'friedman_mse'}</t>
         </is>
       </c>
     </row>
@@ -854,25 +854,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9629629629629629</v>
+        <v>0.683069224353628</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5947712418300654</v>
+        <v>0.575</v>
       </c>
       <c r="D15" t="n">
-        <v>5.209033966064452</v>
+        <v>15.14929246902466</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5599251603706343</v>
+        <v>0.671405160390516</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Meta 25%</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>{'warm_start': True, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': 10, 'criterion': 'gini', 'bootstrap': True}</t>
+          <t>{'verbose': True, 'n_estimators': 50, 'min_weight_fraction_leaf': 0.001, 'min_samples_split': 6, 'min_samples_leaf': 10, 'max_features': 11, 'max_depth': 5, 'loss': 'log_loss', 'learning_rate': 0.1, 'init': 'zero', 'criterion': 'squared_error'}</t>
         </is>
       </c>
     </row>
@@ -883,25 +883,25 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>0.762301918265221</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5816993464052288</v>
+        <v>0.5825</v>
       </c>
       <c r="D16" t="n">
-        <v>6.054723501205444</v>
+        <v>56.70133709907532</v>
       </c>
       <c r="E16" t="n">
-        <v>0.5882573057733428</v>
+        <v>0.6647280334728034</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Meta 25%</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>{'warm_start': True, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': None, 'criterion': 'gini', 'bootstrap': True}</t>
+          <t>{'verbose': True, 'n_estimators': 25, 'min_weight_fraction_leaf': 0.01, 'min_samples_split': 6, 'min_samples_leaf': 5, 'max_features': 5, 'max_depth': 10, 'loss': 'log_loss', 'learning_rate': 0.1, 'init': 'zero', 'criterion': 'friedman_mse'}</t>
         </is>
       </c>
     </row>
@@ -912,74 +912,74 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9662309368191722</v>
+        <v>0.9974979149291076</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5915032679738562</v>
+        <v>0.6525</v>
       </c>
       <c r="D17" t="n">
-        <v>7.224881649017334</v>
+        <v>18.73439025878906</v>
       </c>
       <c r="E17" t="n">
-        <v>0.5861190306486102</v>
+        <v>0.6563877266387727</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Meta 25%</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>{'warm_start': True, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': 10, 'criterion': 'gini', 'bootstrap': True}</t>
+          <t>{'verbose': True, 'n_estimators': 200, 'min_weight_fraction_leaf': 0.01, 'min_samples_split': 4, 'min_samples_leaf': 10, 'max_features': 3, 'max_depth': 5, 'loss': 'log_loss', 'learning_rate': 0.1, 'init': 'zero', 'criterion': 'friedman_mse'}</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GridSearchCV</t>
+          <t>RandomizedSearchCV</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6816326530612244</v>
+        <v>0.6375</v>
       </c>
       <c r="D18" t="n">
-        <v>28.0901460647583</v>
+        <v>2.775870561599731</v>
       </c>
       <c r="E18" t="n">
-        <v>0.6634806947302081</v>
+        <v>0.6355474198047421</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Full_Train_Set</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>{'bootstrap': True, 'criterion': 'entropy', 'max_depth': None, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': True}</t>
+          <t>{'n_estimators': 25, 'min_weight_fraction_leaf': 0.1, 'min_samples_split': 2, 'min_samples_leaf': 1, 'max_features': 7, 'max_depth': 10, 'loss': 'log_loss', 'learning_rate': 0.1, 'init': 'zero', 'criterion': 'squared_error'}</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BayesSearchCV</t>
+          <t>RandomizedSearchCV</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>0.9616346955796498</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6840816326530612</v>
+        <v>0.63</v>
       </c>
       <c r="D19" t="n">
-        <v>72.43652844429016</v>
+        <v>5.135035753250124</v>
       </c>
       <c r="E19" t="n">
-        <v>0.6634810654507034</v>
+        <v>0.5588249651324965</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -988,7 +988,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>OrderedDict([('bootstrap', True), ('criterion', 'entropy'), ('max_depth', None), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', True)])</t>
+          <t>{'n_estimators': 100, 'min_weight_fraction_leaf': 0.1, 'min_samples_split': 4, 'min_samples_leaf': 5, 'max_features': 5, 'max_depth': 10, 'loss': 'log_loss', 'learning_rate': 0.001, 'init': None, 'criterion': 'friedman_mse'}</t>
         </is>
       </c>
     </row>
@@ -999,16 +999,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>0.8490408673894912</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6726530612244898</v>
+        <v>0.605</v>
       </c>
       <c r="D20" t="n">
-        <v>7.861243486404421</v>
+        <v>34.75495028495789</v>
       </c>
       <c r="E20" t="n">
-        <v>0.661845817346012</v>
+        <v>0.6655822873082288</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1017,558 +1017,36 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>{'warm_start': False, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': 25, 'criterion': 'log_loss', 'bootstrap': True}</t>
+          <t>{'n_estimators': 50, 'min_weight_fraction_leaf': 0.001, 'min_samples_split': 4, 'min_samples_leaf': 1, 'max_features': 7, 'max_depth': 10, 'loss': 'log_loss', 'learning_rate': 0.1, 'init': 'zero', 'criterion': 'squared_error'}</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GridSearchCV</t>
+          <t>RandomizedSearchCV</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0.6738949124270225</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5392156862745098</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D21" t="n">
-        <v>15.49386310577393</v>
+        <v>36.26125025749207</v>
       </c>
       <c r="E21" t="n">
-        <v>0.5523342836778331</v>
+        <v>0.671415620641562</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Meta 25%</t>
+          <t>Full Train Set</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>{'bootstrap': True, 'criterion': 'entropy', 'max_depth': 25, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': False}</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>BayesSearchCV</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.9836601307189542</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.5359477124183006</v>
-      </c>
-      <c r="D22" t="n">
-        <v>48.57947373390198</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.5523461629840817</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Meta 25%</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>OrderedDict([('bootstrap', True), ('criterion', 'log_loss'), ('max_depth', 10), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', True)])</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>RandomizedSearchCV</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>0.9520697167755992</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.5359477124183006</v>
-      </c>
-      <c r="D23" t="n">
-        <v>6.242515802383423</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.5501366120218579</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Meta 25%</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>{'warm_start': True, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': 10, 'criterion': 'gini', 'bootstrap': True}</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>GridSearchCV</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.6783673469387755</v>
-      </c>
-      <c r="D24" t="n">
-        <v>28.60687160491943</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.6664787113755584</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Full_Train_Set</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>{'bootstrap': True, 'criterion': 'log_loss', 'max_depth': 25, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': False}</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>BayesSearchCV</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.6808163265306122</v>
-      </c>
-      <c r="D25" t="n">
-        <v>68.99149703979491</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.6629409256890767</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Full Train Set</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>OrderedDict([('bootstrap', True), ('criterion', 'entropy'), ('max_depth', None), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', True)])</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>RandomizedSearchCV</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.6759183673469388</v>
-      </c>
-      <c r="D26" t="n">
-        <v>17.72540378570557</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.6588566979925485</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Full Train Set</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>{'warm_start': True, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': None, 'criterion': 'log_loss', 'bootstrap': True}</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>GridSearchCV</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>0.9673202614379085</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.6274509803921569</v>
-      </c>
-      <c r="D27" t="n">
-        <v>15.36597323417664</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.5926110715134236</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Meta 25%</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>{'bootstrap': True, 'criterion': 'entropy', 'max_depth': 10, 'n_estimators': 25, 'n_jobs': -1, 'warm_start': False}</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>BayesSearchCV</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>0.985838779956427</v>
-      </c>
-      <c r="C28" t="n">
-        <v>0.5915032679738562</v>
-      </c>
-      <c r="D28" t="n">
-        <v>44.38564133644105</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.5904133998574483</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Meta 25%</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>OrderedDict([('bootstrap', True), ('criterion', 'log_loss'), ('max_depth', 10), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', True)])</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>RandomizedSearchCV</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>0.9814814814814815</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.5816993464052288</v>
-      </c>
-      <c r="D29" t="n">
-        <v>5.492424964904785</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.5827868852459016</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Meta 25%</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>{'warm_start': True, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': 10, 'criterion': 'log_loss', 'bootstrap': True}</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>RandomizedSearchCV</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0.6702040816326531</v>
-      </c>
-      <c r="D30" t="n">
-        <v>14.03323125839233</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.6547746946189921</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Full Train Set</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>{'warm_start': True, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': None, 'criterion': 'gini', 'bootstrap': True}</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>GridSearchCV</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>0.9825708061002179</v>
-      </c>
-      <c r="C31" t="n">
-        <v>0.5555555555555556</v>
-      </c>
-      <c r="D31" t="n">
-        <v>15.45255494117737</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0.55664053219292</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Meta 25%</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>{'bootstrap': True, 'criterion': 'log_loss', 'max_depth': 10, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': False}</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>BayesSearchCV</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" t="n">
-        <v>0.5555555555555556</v>
-      </c>
-      <c r="D32" t="n">
-        <v>41.5915606021881</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.5566108339272987</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Meta 25%</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>OrderedDict([('bootstrap', False), ('criterion', 'gini'), ('max_depth', 25), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', True)])</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>RandomizedSearchCV</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>0.9673202614379085</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0.5555555555555556</v>
-      </c>
-      <c r="D33" t="n">
-        <v>4.443576812744141</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0.5511582323592302</v>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Meta 25%</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>{'warm_start': False, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': 10, 'criterion': 'gini', 'bootstrap': False}</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>GridSearchCV</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0.6775510204081633</v>
-      </c>
-      <c r="D34" t="n">
-        <v>33.11461615562439</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.66402750746075</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Full_Train_Set</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>{'bootstrap': True, 'criterion': 'log_loss', 'max_depth': 25, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': False}</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>BayesSearchCV</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0.686530612244898</v>
-      </c>
-      <c r="D35" t="n">
-        <v>81.07771182060242</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.6653880516784371</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Full Train Set</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>OrderedDict([('bootstrap', True), ('criterion', 'log_loss'), ('max_depth', 25), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', False)])</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>RandomizedSearchCV</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0.6718367346938775</v>
-      </c>
-      <c r="D36" t="n">
-        <v>23.89962220191956</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.661851007432946</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Full Train Set</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>{'warm_start': False, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': None, 'criterion': 'entropy', 'bootstrap': True}</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>GridSearchCV</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" t="n">
-        <v>0.5588235294117647</v>
-      </c>
-      <c r="D37" t="n">
-        <v>39.22216987609864</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0.5784271798526965</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Meta 25%</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>{'bootstrap': False, 'criterion': 'entropy', 'max_depth': None, 'n_estimators': 100, 'n_jobs': -1, 'warm_start': True}</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>BayesSearchCV</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>0.9836601307189542</v>
-      </c>
-      <c r="C38" t="n">
-        <v>0.5816993464052288</v>
-      </c>
-      <c r="D38" t="n">
-        <v>49.93530178070068</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0.579543834640057</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Meta 25%</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>OrderedDict([('bootstrap', True), ('criterion', 'entropy'), ('max_depth', 10), ('n_estimators', 100), ('n_jobs', -1), ('warm_start', False)])</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>RandomizedSearchCV</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" t="n">
-        <v>0.5947712418300654</v>
-      </c>
-      <c r="D39" t="n">
-        <v>4.656710624694824</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0.5729864575908767</v>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Meta 25%</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>{'warm_start': False, 'n_jobs': -1, 'n_estimators': 100, 'max_depth': 25, 'criterion': 'gini', 'bootstrap': True}</t>
+          <t>{'n_estimators': 100, 'min_weight_fraction_leaf': 0.001, 'min_samples_split': 6, 'min_samples_leaf': 1, 'max_features': 3, 'max_depth': 5, 'loss': 'log_loss', 'learning_rate': 0.1, 'init': None, 'criterion': 'friedman_mse'}</t>
         </is>
       </c>
     </row>

</xml_diff>